<commit_message>
Try to fix ScrollView, failed
</commit_message>
<xml_diff>
--- a/_DESIGN/formulas.xlsx
+++ b/_DESIGN/formulas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11415" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11415" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet4!$A$1:$D$1</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="74">
   <si>
     <t>&lt;LinearLayout                 android:layout_width="&amp;char(34)&amp;"match_parent"&amp;char(34)&amp;"                 android:layout_height="&amp;char(34)&amp;"match_parent"&amp;char(34)&amp;"                 android:orientation="&amp;char(34)&amp;"horizontal"&amp;char(34)&amp;"&gt;                  &lt;TextView                     android:id="&amp;char(34)&amp;"@+id/textView4"&amp;char(34)&amp;"                     android:layout_width="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                     android:layout_height="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                     android:layout_weight="&amp;char(34)&amp;"1"&amp;char(34)&amp;"                     android:text="&amp;char(34)&amp;"1."&amp;char(34)&amp;" /&gt;                  &lt;TextView                     android:id="&amp;char(34)&amp;"@+id/textView3"&amp;char(34)&amp;"                     android:layout_width="&amp;char(34)&amp;"183dp"&amp;char(34)&amp;"                     android:layout_height="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                     android:layout_weight="&amp;char(34)&amp;"1"&amp;char(34)&amp;"                     android:text="&amp;char(34)&amp;"TextView"&amp;char(34)&amp;" /&gt;                  &lt;RadioGroup                     android:layout_width="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                     android:layout_height="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                     android:layout_weight="&amp;char(34)&amp;"1"&amp;char(34)&amp;"                     android:orientation="&amp;char(34)&amp;"horizontal"&amp;char(34)&amp;"&gt;                      &lt;RadioButton                         android:id="&amp;char(34)&amp;"@+id/radioButton"&amp;char(34)&amp;"                         android:layout_width="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                         android:layout_height="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                         android:layout_weight="&amp;char(34)&amp;"1"&amp;char(34)&amp;" /&gt;                      &lt;RadioButton                         android:id="&amp;char(34)&amp;"@+id/radioButton2"&amp;char(34)&amp;"                         android:layout_width="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                         android:layout_height="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                         android:layout_weight="&amp;char(34)&amp;"1"&amp;char(34)&amp;" /&gt;                      &lt;RadioButton                         android:id="&amp;char(34)&amp;"@+id/radioButton3"&amp;char(34)&amp;"                         android:layout_width="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                         android:layout_height="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                         android:layout_weight="&amp;char(34)&amp;"1"&amp;char(34)&amp;" /&gt;                      &lt;RadioButton                         android:id="&amp;char(34)&amp;"@+id/radioButton4"&amp;char(34)&amp;"                         android:layout_width="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                         android:layout_height="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                         android:layout_weight="&amp;char(34)&amp;"1"&amp;char(34)&amp;" /&gt;                      &lt;RadioButton                         android:id="&amp;char(34)&amp;"@+id/radioButton5"&amp;char(34)&amp;"                         android:layout_width="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                         android:layout_height="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                         android:layout_weight="&amp;char(34)&amp;"1"&amp;char(34)&amp;" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</t>
   </si>
@@ -250,6 +251,9 @@
   </si>
   <si>
     <t>r</t>
+  </si>
+  <si>
+    <t>if (question50radioButton1.isChecked()) answers[50]=1; else if (question50radioButton2.isChecked()) answers[50]=2; else if (question50radioButton3.isChecked()) answers[50]=3; else if (question50radioButton4.isChecked()) answers[50]=4; else if (question50radioButton5.isChecked()) answers[50]=5; else { notCompleted(50, layout50); return; }</t>
   </si>
 </sst>
 </file>
@@ -2064,7 +2068,7 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="C1" sqref="C1:C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2080,8 +2084,8 @@
         <v>7</v>
       </c>
       <c r="C1" t="str">
-        <f>"&lt;LinearLayout                 android:layout_width="&amp;CHAR(34)&amp;"match_parent"&amp;CHAR(34)&amp;"                 android:layout_height="&amp;CHAR(34)&amp;"match_parent"&amp;CHAR(34)&amp;"                 android:orientation="&amp;CHAR(34)&amp;"horizontal"&amp;CHAR(34)&amp;"android:gravity="&amp;CHAR(34)&amp;"center_vertical"&amp;CHAR(34)&amp;"                 android:layout_marginTop="&amp;CHAR(34)&amp;"4dp"&amp;CHAR(34)&amp;"                 android:layout_marginBottom="&amp;CHAR(34)&amp;"4dp"&amp;CHAR(34)&amp;"&gt;                  &lt;TextView                     android:id="&amp;CHAR(34)&amp;"@+id/label"&amp;A1&amp;CHAR(34)&amp;"                     android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                     android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                     android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;"                     android:text="&amp;CHAR(34)&amp;A1&amp;"."&amp;CHAR(34)&amp;" /&gt;                  &lt;TextView                     android:id="&amp;CHAR(34)&amp;"@+id/question"&amp;A1&amp;CHAR(34)&amp;"                     android:layout_width="&amp;CHAR(34)&amp;"183dp"&amp;CHAR(34)&amp;"                     android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                     android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;"                     android:text="&amp;CHAR(34)&amp;B1&amp;CHAR(34)&amp;" /&gt;                  &lt;RadioGroup                     android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                     android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                     android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;"                     android:orientation="&amp;CHAR(34)&amp;"horizontal"&amp;CHAR(34)&amp;"&gt;                      &lt;RadioButton                         android:id="&amp;CHAR(34)&amp;"@+id/question"&amp;A1&amp;"radioButton1"&amp;CHAR(34)&amp;"                         android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" /&gt;                      &lt;RadioButton                         android:id="&amp;CHAR(34)&amp;"@+id/question"&amp;A1&amp;"radioButton2"&amp;CHAR(34)&amp;"                         android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" /&gt;                      &lt;RadioButton                         android:id="&amp;CHAR(34)&amp;"@+id/question"&amp;A1&amp;"radioButton3"&amp;CHAR(34)&amp;"                         android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" /&gt;                      &lt;RadioButton                         android:id="&amp;CHAR(34)&amp;"@+id/question"&amp;A1&amp;"radioButton4"&amp;CHAR(34)&amp;"                         android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" /&gt;                      &lt;RadioButton                         android:id="&amp;CHAR(34)&amp;"@+id/question"&amp;A1&amp;"radioButton5"&amp;CHAR(34)&amp;"                         android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;"</f>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label1"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="1." /&gt;                  &lt;TextView                     android:id="@+id/question1"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Am the life of the party." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question1radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question1radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question1radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question1radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question1radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <f>"&lt;LinearLayout                 android:id="&amp;CHAR(34)&amp;"@+id/layout"&amp;A1&amp;CHAR(34)&amp;"                 android:layout_width="&amp;CHAR(34)&amp;"match_parent"&amp;CHAR(34)&amp;"                 android:layout_height="&amp;CHAR(34)&amp;"match_parent"&amp;CHAR(34)&amp;"                 android:orientation="&amp;CHAR(34)&amp;"horizontal"&amp;CHAR(34)&amp;"android:gravity="&amp;CHAR(34)&amp;"center_vertical"&amp;CHAR(34)&amp;"                 android:layout_marginTop="&amp;CHAR(34)&amp;"4dp"&amp;CHAR(34)&amp;"                 android:layout_marginBottom="&amp;CHAR(34)&amp;"4dp"&amp;CHAR(34)&amp;"&gt;                  &lt;TextView                     android:id="&amp;CHAR(34)&amp;"@+id/label"&amp;A1&amp;CHAR(34)&amp;"                     android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                     android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                     android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;"                     android:text="&amp;CHAR(34)&amp;A1&amp;"."&amp;CHAR(34)&amp;" /&gt;                  &lt;TextView                     android:id="&amp;CHAR(34)&amp;"@+id/question"&amp;A1&amp;CHAR(34)&amp;"                     android:layout_width="&amp;CHAR(34)&amp;"183dp"&amp;CHAR(34)&amp;"                     android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                     android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;"                     android:text="&amp;CHAR(34)&amp;B1&amp;CHAR(34)&amp;" /&gt;                  &lt;RadioGroup                     android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                     android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                     android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;"                     android:orientation="&amp;CHAR(34)&amp;"horizontal"&amp;CHAR(34)&amp;"&gt;                      &lt;RadioButton                         android:id="&amp;CHAR(34)&amp;"@+id/question"&amp;A1&amp;"radioButton1"&amp;CHAR(34)&amp;"                         android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" /&gt;                      &lt;RadioButton                         android:id="&amp;CHAR(34)&amp;"@+id/question"&amp;A1&amp;"radioButton2"&amp;CHAR(34)&amp;"                         android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" /&gt;                      &lt;RadioButton                         android:id="&amp;CHAR(34)&amp;"@+id/question"&amp;A1&amp;"radioButton3"&amp;CHAR(34)&amp;"                         android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" /&gt;                      &lt;RadioButton                         android:id="&amp;CHAR(34)&amp;"@+id/question"&amp;A1&amp;"radioButton4"&amp;CHAR(34)&amp;"                         android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" /&gt;                      &lt;RadioButton                         android:id="&amp;CHAR(34)&amp;"@+id/question"&amp;A1&amp;"radioButton5"&amp;CHAR(34)&amp;"                         android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;"</f>
+        <v>&lt;LinearLayout                 android:id="@+id/layout1"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label1"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="1." /&gt;                  &lt;TextView                     android:id="@+id/question1"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Am the life of the party." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question1radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question1radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question1radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question1radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question1radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2092,8 +2096,8 @@
         <v>10</v>
       </c>
       <c r="C2" t="str">
-        <f t="shared" ref="C2:C50" si="0">"&lt;LinearLayout                 android:layout_width="&amp;CHAR(34)&amp;"match_parent"&amp;CHAR(34)&amp;"                 android:layout_height="&amp;CHAR(34)&amp;"match_parent"&amp;CHAR(34)&amp;"                 android:orientation="&amp;CHAR(34)&amp;"horizontal"&amp;CHAR(34)&amp;"android:gravity="&amp;CHAR(34)&amp;"center_vertical"&amp;CHAR(34)&amp;"                 android:layout_marginTop="&amp;CHAR(34)&amp;"4dp"&amp;CHAR(34)&amp;"                 android:layout_marginBottom="&amp;CHAR(34)&amp;"4dp"&amp;CHAR(34)&amp;"&gt;                  &lt;TextView                     android:id="&amp;CHAR(34)&amp;"@+id/label"&amp;A2&amp;CHAR(34)&amp;"                     android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                     android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                     android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;"                     android:text="&amp;CHAR(34)&amp;A2&amp;"."&amp;CHAR(34)&amp;" /&gt;                  &lt;TextView                     android:id="&amp;CHAR(34)&amp;"@+id/question"&amp;A2&amp;CHAR(34)&amp;"                     android:layout_width="&amp;CHAR(34)&amp;"183dp"&amp;CHAR(34)&amp;"                     android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                     android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;"                     android:text="&amp;CHAR(34)&amp;B2&amp;CHAR(34)&amp;" /&gt;                  &lt;RadioGroup                     android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                     android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                     android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;"                     android:orientation="&amp;CHAR(34)&amp;"horizontal"&amp;CHAR(34)&amp;"&gt;                      &lt;RadioButton                         android:id="&amp;CHAR(34)&amp;"@+id/question"&amp;A2&amp;"radioButton1"&amp;CHAR(34)&amp;"                         android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" /&gt;                      &lt;RadioButton                         android:id="&amp;CHAR(34)&amp;"@+id/question"&amp;A2&amp;"radioButton2"&amp;CHAR(34)&amp;"                         android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" /&gt;                      &lt;RadioButton                         android:id="&amp;CHAR(34)&amp;"@+id/question"&amp;A2&amp;"radioButton3"&amp;CHAR(34)&amp;"                         android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" /&gt;                      &lt;RadioButton                         android:id="&amp;CHAR(34)&amp;"@+id/question"&amp;A2&amp;"radioButton4"&amp;CHAR(34)&amp;"                         android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" /&gt;                      &lt;RadioButton                         android:id="&amp;CHAR(34)&amp;"@+id/question"&amp;A2&amp;"radioButton5"&amp;CHAR(34)&amp;"                         android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;"</f>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label2"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="2." /&gt;                  &lt;TextView                     android:id="@+id/question2"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Feel little concern for others." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question2radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question2radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question2radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question2radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question2radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <f t="shared" ref="C2:C50" si="0">"&lt;LinearLayout                 android:id="&amp;CHAR(34)&amp;"@+id/layout"&amp;A2&amp;CHAR(34)&amp;"                 android:layout_width="&amp;CHAR(34)&amp;"match_parent"&amp;CHAR(34)&amp;"                 android:layout_height="&amp;CHAR(34)&amp;"match_parent"&amp;CHAR(34)&amp;"                 android:orientation="&amp;CHAR(34)&amp;"horizontal"&amp;CHAR(34)&amp;"android:gravity="&amp;CHAR(34)&amp;"center_vertical"&amp;CHAR(34)&amp;"                 android:layout_marginTop="&amp;CHAR(34)&amp;"4dp"&amp;CHAR(34)&amp;"                 android:layout_marginBottom="&amp;CHAR(34)&amp;"4dp"&amp;CHAR(34)&amp;"&gt;                  &lt;TextView                     android:id="&amp;CHAR(34)&amp;"@+id/label"&amp;A2&amp;CHAR(34)&amp;"                     android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                     android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                     android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;"                     android:text="&amp;CHAR(34)&amp;A2&amp;"."&amp;CHAR(34)&amp;" /&gt;                  &lt;TextView                     android:id="&amp;CHAR(34)&amp;"@+id/question"&amp;A2&amp;CHAR(34)&amp;"                     android:layout_width="&amp;CHAR(34)&amp;"183dp"&amp;CHAR(34)&amp;"                     android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                     android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;"                     android:text="&amp;CHAR(34)&amp;B2&amp;CHAR(34)&amp;" /&gt;                  &lt;RadioGroup                     android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                     android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                     android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;"                     android:orientation="&amp;CHAR(34)&amp;"horizontal"&amp;CHAR(34)&amp;"&gt;                      &lt;RadioButton                         android:id="&amp;CHAR(34)&amp;"@+id/question"&amp;A2&amp;"radioButton1"&amp;CHAR(34)&amp;"                         android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" /&gt;                      &lt;RadioButton                         android:id="&amp;CHAR(34)&amp;"@+id/question"&amp;A2&amp;"radioButton2"&amp;CHAR(34)&amp;"                         android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" /&gt;                      &lt;RadioButton                         android:id="&amp;CHAR(34)&amp;"@+id/question"&amp;A2&amp;"radioButton3"&amp;CHAR(34)&amp;"                         android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" /&gt;                      &lt;RadioButton                         android:id="&amp;CHAR(34)&amp;"@+id/question"&amp;A2&amp;"radioButton4"&amp;CHAR(34)&amp;"                         android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" /&gt;                      &lt;RadioButton                         android:id="&amp;CHAR(34)&amp;"@+id/question"&amp;A2&amp;"radioButton5"&amp;CHAR(34)&amp;"                         android:layout_width="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_height="&amp;CHAR(34)&amp;"wrap_content"&amp;CHAR(34)&amp;"                         android:layout_weight="&amp;CHAR(34)&amp;"1"&amp;CHAR(34)&amp;" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;"</f>
+        <v>&lt;LinearLayout                 android:id="@+id/layout2"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label2"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="2." /&gt;                  &lt;TextView                     android:id="@+id/question2"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Feel little concern for others." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question2radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question2radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question2radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question2radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question2radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2105,7 +2109,7 @@
       </c>
       <c r="C3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label3"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="3." /&gt;                  &lt;TextView                     android:id="@+id/question3"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Am always prepared." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question3radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question3radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question3radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question3radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question3radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout3"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label3"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="3." /&gt;                  &lt;TextView                     android:id="@+id/question3"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Am always prepared." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question3radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question3radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question3radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question3radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question3radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2117,7 +2121,7 @@
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label4"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="4." /&gt;                  &lt;TextView                     android:id="@+id/question4"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Get stressed out easily." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question4radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question4radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question4radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question4radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question4radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout4"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label4"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="4." /&gt;                  &lt;TextView                     android:id="@+id/question4"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Get stressed out easily." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question4radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question4radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question4radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question4radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question4radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2129,7 +2133,7 @@
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label5"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="5." /&gt;                  &lt;TextView                     android:id="@+id/question5"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Have a rich vocabulary." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question5radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question5radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question5radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question5radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question5radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout5"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label5"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="5." /&gt;                  &lt;TextView                     android:id="@+id/question5"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Have a rich vocabulary." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question5radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question5radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question5radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question5radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question5radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2141,7 +2145,7 @@
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label6"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="6." /&gt;                  &lt;TextView                     android:id="@+id/question6"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Don't talk a lot." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question6radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question6radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question6radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question6radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question6radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout6"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label6"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="6." /&gt;                  &lt;TextView                     android:id="@+id/question6"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Don't talk a lot." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question6radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question6radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question6radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question6radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question6radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2153,7 +2157,7 @@
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label7"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="7." /&gt;                  &lt;TextView                     android:id="@+id/question7"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Am interested in people." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question7radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question7radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question7radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question7radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question7radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout7"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label7"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="7." /&gt;                  &lt;TextView                     android:id="@+id/question7"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Am interested in people." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question7radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question7radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question7radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question7radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question7radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2165,7 +2169,7 @@
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label8"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="8." /&gt;                  &lt;TextView                     android:id="@+id/question8"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Leave my belongings around." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question8radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question8radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question8radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question8radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question8radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout8"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label8"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="8." /&gt;                  &lt;TextView                     android:id="@+id/question8"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Leave my belongings around." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question8radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question8radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question8radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question8radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question8radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2177,7 +2181,7 @@
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label9"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="9." /&gt;                  &lt;TextView                     android:id="@+id/question9"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Am relaxed most of the time." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question9radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question9radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question9radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question9radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question9radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout9"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label9"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="9." /&gt;                  &lt;TextView                     android:id="@+id/question9"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Am relaxed most of the time." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question9radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question9radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question9radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question9radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question9radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2189,7 +2193,7 @@
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label10"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="10." /&gt;                  &lt;TextView                     android:id="@+id/question10"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Have difficulty understanding abstract ideas." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question10radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question10radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question10radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question10radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question10radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout10"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label10"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="10." /&gt;                  &lt;TextView                     android:id="@+id/question10"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Have difficulty understanding abstract ideas." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question10radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question10radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question10radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question10radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question10radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2201,7 +2205,7 @@
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label11"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="11." /&gt;                  &lt;TextView                     android:id="@+id/question11"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Feel comfortable around people." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question11radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question11radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question11radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question11radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question11radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout11"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label11"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="11." /&gt;                  &lt;TextView                     android:id="@+id/question11"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Feel comfortable around people." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question11radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question11radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question11radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question11radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question11radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2213,7 +2217,7 @@
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label12"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="12." /&gt;                  &lt;TextView                     android:id="@+id/question12"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Insult people." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question12radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question12radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question12radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question12radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question12radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout12"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label12"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="12." /&gt;                  &lt;TextView                     android:id="@+id/question12"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Insult people." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question12radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question12radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question12radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question12radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question12radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2225,7 +2229,7 @@
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label13"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="13." /&gt;                  &lt;TextView                     android:id="@+id/question13"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Pay attention to details." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question13radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question13radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question13radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question13radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question13radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout13"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label13"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="13." /&gt;                  &lt;TextView                     android:id="@+id/question13"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Pay attention to details." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question13radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question13radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question13radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question13radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question13radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2237,7 +2241,7 @@
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label14"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="14." /&gt;                  &lt;TextView                     android:id="@+id/question14"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Worry about things." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question14radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question14radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question14radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question14radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question14radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout14"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label14"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="14." /&gt;                  &lt;TextView                     android:id="@+id/question14"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Worry about things." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question14radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question14radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question14radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question14radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question14radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2249,7 +2253,7 @@
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label15"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="15." /&gt;                  &lt;TextView                     android:id="@+id/question15"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Have a vivid imagination." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question15radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question15radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question15radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question15radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question15radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout15"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label15"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="15." /&gt;                  &lt;TextView                     android:id="@+id/question15"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Have a vivid imagination." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question15radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question15radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question15radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question15radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question15radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2261,7 +2265,7 @@
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label16"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="16." /&gt;                  &lt;TextView                     android:id="@+id/question16"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Keep in the background." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question16radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question16radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question16radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question16radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question16radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout16"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label16"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="16." /&gt;                  &lt;TextView                     android:id="@+id/question16"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Keep in the background." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question16radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question16radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question16radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question16radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question16radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2273,7 +2277,7 @@
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label17"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="17." /&gt;                  &lt;TextView                     android:id="@+id/question17"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Sympathize with others' feelings." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question17radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question17radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question17radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question17radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question17radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout17"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label17"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="17." /&gt;                  &lt;TextView                     android:id="@+id/question17"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Sympathize with others' feelings." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question17radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question17radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question17radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question17radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question17radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2285,7 +2289,7 @@
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label18"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="18." /&gt;                  &lt;TextView                     android:id="@+id/question18"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Make a mess of things." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question18radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question18radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question18radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question18radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question18radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout18"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label18"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="18." /&gt;                  &lt;TextView                     android:id="@+id/question18"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Make a mess of things." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question18radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question18radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question18radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question18radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question18radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2297,7 +2301,7 @@
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label19"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="19." /&gt;                  &lt;TextView                     android:id="@+id/question19"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Seldom feel blue." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question19radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question19radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question19radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question19radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question19radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout19"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label19"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="19." /&gt;                  &lt;TextView                     android:id="@+id/question19"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Seldom feel blue." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question19radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question19radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question19radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question19radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question19radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2309,7 +2313,7 @@
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label20"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="20." /&gt;                  &lt;TextView                     android:id="@+id/question20"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Am not interested in abstract ideas." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question20radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question20radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question20radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question20radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question20radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout20"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label20"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="20." /&gt;                  &lt;TextView                     android:id="@+id/question20"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Am not interested in abstract ideas." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question20radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question20radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question20radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question20radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question20radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2321,7 +2325,7 @@
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label21"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="21." /&gt;                  &lt;TextView                     android:id="@+id/question21"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Start conversations." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question21radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question21radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question21radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question21radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question21radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout21"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label21"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="21." /&gt;                  &lt;TextView                     android:id="@+id/question21"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Start conversations." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question21radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question21radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question21radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question21radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question21radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2333,7 +2337,7 @@
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label22"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="22." /&gt;                  &lt;TextView                     android:id="@+id/question22"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Am not interested in other people's problems." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question22radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question22radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question22radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question22radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question22radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout22"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label22"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="22." /&gt;                  &lt;TextView                     android:id="@+id/question22"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Am not interested in other people's problems." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question22radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question22radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question22radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question22radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question22radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2345,7 +2349,7 @@
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label23"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="23." /&gt;                  &lt;TextView                     android:id="@+id/question23"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Get chores done right away." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question23radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question23radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question23radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question23radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question23radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout23"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label23"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="23." /&gt;                  &lt;TextView                     android:id="@+id/question23"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Get chores done right away." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question23radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question23radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question23radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question23radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question23radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2357,7 +2361,7 @@
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label24"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="24." /&gt;                  &lt;TextView                     android:id="@+id/question24"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Am easily disturbed." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question24radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question24radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question24radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question24radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question24radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout24"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label24"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="24." /&gt;                  &lt;TextView                     android:id="@+id/question24"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Am easily disturbed." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question24radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question24radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question24radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question24radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question24radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2369,7 +2373,7 @@
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label25"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="25." /&gt;                  &lt;TextView                     android:id="@+id/question25"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Have excellent ideas." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question25radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question25radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question25radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question25radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question25radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout25"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label25"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="25." /&gt;                  &lt;TextView                     android:id="@+id/question25"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Have excellent ideas." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question25radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question25radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question25radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question25radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question25radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2381,7 +2385,7 @@
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label26"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="26." /&gt;                  &lt;TextView                     android:id="@+id/question26"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Have little to say." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question26radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question26radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question26radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question26radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question26radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout26"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label26"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="26." /&gt;                  &lt;TextView                     android:id="@+id/question26"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Have little to say." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question26radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question26radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question26radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question26radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question26radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2393,7 +2397,7 @@
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label27"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="27." /&gt;                  &lt;TextView                     android:id="@+id/question27"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Have a soft heart." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question27radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question27radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question27radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question27radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question27radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout27"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label27"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="27." /&gt;                  &lt;TextView                     android:id="@+id/question27"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Have a soft heart." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question27radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question27radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question27radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question27radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question27radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2405,7 +2409,7 @@
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label28"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="28." /&gt;                  &lt;TextView                     android:id="@+id/question28"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Often forget to put things back in their proper place." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question28radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question28radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question28radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question28radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question28radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout28"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label28"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="28." /&gt;                  &lt;TextView                     android:id="@+id/question28"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Often forget to put things back in their proper place." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question28radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question28radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question28radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question28radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question28radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2417,7 +2421,7 @@
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label29"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="29." /&gt;                  &lt;TextView                     android:id="@+id/question29"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Get upset easily." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question29radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question29radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question29radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question29radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question29radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout29"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label29"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="29." /&gt;                  &lt;TextView                     android:id="@+id/question29"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Get upset easily." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question29radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question29radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question29radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question29radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question29radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2429,7 +2433,7 @@
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label30"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="30." /&gt;                  &lt;TextView                     android:id="@+id/question30"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Do not have a good imagination." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question30radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question30radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question30radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question30radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question30radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout30"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label30"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="30." /&gt;                  &lt;TextView                     android:id="@+id/question30"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Do not have a good imagination." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question30radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question30radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question30radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question30radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question30radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2441,7 +2445,7 @@
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label31"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="31." /&gt;                  &lt;TextView                     android:id="@+id/question31"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Talk to a lot of different people at parties." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question31radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question31radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question31radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question31radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question31radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout31"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label31"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="31." /&gt;                  &lt;TextView                     android:id="@+id/question31"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Talk to a lot of different people at parties." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question31radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question31radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question31radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question31radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question31radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2453,7 +2457,7 @@
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label32"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="32." /&gt;                  &lt;TextView                     android:id="@+id/question32"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Am not really interested in others." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question32radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question32radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question32radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question32radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question32radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout32"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label32"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="32." /&gt;                  &lt;TextView                     android:id="@+id/question32"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Am not really interested in others." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question32radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question32radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question32radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question32radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question32radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2465,7 +2469,7 @@
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label33"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="33." /&gt;                  &lt;TextView                     android:id="@+id/question33"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Like order." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question33radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question33radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question33radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question33radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question33radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout33"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label33"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="33." /&gt;                  &lt;TextView                     android:id="@+id/question33"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Like order." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question33radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question33radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question33radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question33radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question33radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2477,7 +2481,7 @@
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label34"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="34." /&gt;                  &lt;TextView                     android:id="@+id/question34"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Change my mood a lot." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question34radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question34radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question34radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question34radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question34radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout34"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label34"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="34." /&gt;                  &lt;TextView                     android:id="@+id/question34"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Change my mood a lot." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question34radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question34radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question34radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question34radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question34radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -2489,7 +2493,7 @@
       </c>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label35"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="35." /&gt;                  &lt;TextView                     android:id="@+id/question35"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Am quick to understand things." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question35radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question35radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question35radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question35radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question35radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout35"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label35"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="35." /&gt;                  &lt;TextView                     android:id="@+id/question35"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Am quick to understand things." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question35radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question35radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question35radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question35radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question35radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -2501,7 +2505,7 @@
       </c>
       <c r="C36" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label36"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="36." /&gt;                  &lt;TextView                     android:id="@+id/question36"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Don't like to draw attention to myself." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question36radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question36radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question36radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question36radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question36radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout36"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label36"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="36." /&gt;                  &lt;TextView                     android:id="@+id/question36"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Don't like to draw attention to myself." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question36radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question36radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question36radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question36radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question36radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -2513,7 +2517,7 @@
       </c>
       <c r="C37" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label37"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="37." /&gt;                  &lt;TextView                     android:id="@+id/question37"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Take time out for others." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question37radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question37radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question37radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question37radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question37radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout37"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label37"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="37." /&gt;                  &lt;TextView                     android:id="@+id/question37"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Take time out for others." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question37radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question37radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question37radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question37radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question37radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -2525,7 +2529,7 @@
       </c>
       <c r="C38" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label38"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="38." /&gt;                  &lt;TextView                     android:id="@+id/question38"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Shirk my duties." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question38radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question38radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question38radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question38radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question38radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout38"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label38"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="38." /&gt;                  &lt;TextView                     android:id="@+id/question38"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Shirk my duties." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question38radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question38radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question38radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question38radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question38radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -2537,7 +2541,7 @@
       </c>
       <c r="C39" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label39"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="39." /&gt;                  &lt;TextView                     android:id="@+id/question39"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Have frequent mood swings." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question39radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question39radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question39radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question39radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question39radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout39"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label39"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="39." /&gt;                  &lt;TextView                     android:id="@+id/question39"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Have frequent mood swings." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question39radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question39radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question39radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question39radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question39radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -2549,7 +2553,7 @@
       </c>
       <c r="C40" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label40"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="40." /&gt;                  &lt;TextView                     android:id="@+id/question40"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Use difficult words." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question40radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question40radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question40radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question40radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question40radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout40"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label40"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="40." /&gt;                  &lt;TextView                     android:id="@+id/question40"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Use difficult words." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question40radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question40radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question40radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question40radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question40radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -2561,7 +2565,7 @@
       </c>
       <c r="C41" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label41"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="41." /&gt;                  &lt;TextView                     android:id="@+id/question41"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Don't mind being the center of attention." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question41radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question41radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question41radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question41radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question41radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout41"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label41"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="41." /&gt;                  &lt;TextView                     android:id="@+id/question41"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Don't mind being the center of attention." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question41radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question41radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question41radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question41radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question41radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -2573,7 +2577,7 @@
       </c>
       <c r="C42" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label42"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="42." /&gt;                  &lt;TextView                     android:id="@+id/question42"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Feel others' emotions." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question42radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question42radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question42radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question42radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question42radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout42"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label42"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="42." /&gt;                  &lt;TextView                     android:id="@+id/question42"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Feel others' emotions." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question42radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question42radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question42radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question42radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question42radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -2585,7 +2589,7 @@
       </c>
       <c r="C43" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label43"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="43." /&gt;                  &lt;TextView                     android:id="@+id/question43"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Follow a schedule." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question43radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question43radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question43radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question43radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question43radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout43"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label43"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="43." /&gt;                  &lt;TextView                     android:id="@+id/question43"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Follow a schedule." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question43radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question43radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question43radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question43radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question43radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -2597,7 +2601,7 @@
       </c>
       <c r="C44" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label44"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="44." /&gt;                  &lt;TextView                     android:id="@+id/question44"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Get irritated easily." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question44radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question44radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question44radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question44radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question44radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout44"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label44"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="44." /&gt;                  &lt;TextView                     android:id="@+id/question44"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Get irritated easily." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question44radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question44radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question44radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question44radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question44radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -2609,7 +2613,7 @@
       </c>
       <c r="C45" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label45"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="45." /&gt;                  &lt;TextView                     android:id="@+id/question45"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Spend time reflecting on things." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question45radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question45radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question45radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question45radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question45radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout45"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label45"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="45." /&gt;                  &lt;TextView                     android:id="@+id/question45"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Spend time reflecting on things." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question45radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question45radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question45radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question45radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question45radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -2621,7 +2625,7 @@
       </c>
       <c r="C46" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label46"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="46." /&gt;                  &lt;TextView                     android:id="@+id/question46"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Am quiet around strangers." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question46radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question46radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question46radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question46radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question46radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout46"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label46"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="46." /&gt;                  &lt;TextView                     android:id="@+id/question46"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Am quiet around strangers." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question46radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question46radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question46radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question46radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question46radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -2633,7 +2637,7 @@
       </c>
       <c r="C47" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label47"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="47." /&gt;                  &lt;TextView                     android:id="@+id/question47"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Make people feel at ease." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question47radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question47radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question47radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question47radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question47radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout47"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label47"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="47." /&gt;                  &lt;TextView                     android:id="@+id/question47"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Make people feel at ease." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question47radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question47radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question47radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question47radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question47radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -2645,7 +2649,7 @@
       </c>
       <c r="C48" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label48"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="48." /&gt;                  &lt;TextView                     android:id="@+id/question48"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Am exacting in my work." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question48radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question48radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question48radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question48radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question48radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout48"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label48"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="48." /&gt;                  &lt;TextView                     android:id="@+id/question48"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Am exacting in my work." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question48radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question48radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question48radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question48radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question48radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -2657,7 +2661,7 @@
       </c>
       <c r="C49" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label49"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="49." /&gt;                  &lt;TextView                     android:id="@+id/question49"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Often feel blue." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question49radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question49radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question49radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question49radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question49radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout49"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label49"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="49." /&gt;                  &lt;TextView                     android:id="@+id/question49"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Often feel blue." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question49radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question49radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question49radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question49radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question49radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -2669,7 +2673,7 @@
       </c>
       <c r="C50" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;LinearLayout                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label50"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="50." /&gt;                  &lt;TextView                     android:id="@+id/question50"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Am full of ideas." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question50radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question50radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question50radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question50radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question50radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
+        <v>&lt;LinearLayout                 android:id="@+id/layout50"                 android:layout_width="match_parent"                 android:layout_height="match_parent"                 android:orientation="horizontal"android:gravity="center_vertical"                 android:layout_marginTop="4dp"                 android:layout_marginBottom="4dp"&gt;                  &lt;TextView                     android:id="@+id/label50"                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="50." /&gt;                  &lt;TextView                     android:id="@+id/question50"                     android:layout_width="183dp"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:text="Am full of ideas." /&gt;                  &lt;RadioGroup                     android:layout_width="wrap_content"                     android:layout_height="wrap_content"                     android:layout_weight="1"                     android:orientation="horizontal"&gt;                      &lt;RadioButton                         android:id="@+id/question50radioButton1"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question50radioButton2"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question50radioButton3"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question50radioButton4"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                      &lt;RadioButton                         android:id="@+id/question50radioButton5"                         android:layout_width="wrap_content"                         android:layout_height="wrap_content"                         android:layout_weight="1" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</v>
       </c>
     </row>
   </sheetData>
@@ -9271,265 +9275,1337 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A50"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="str">
+        <f>"if (question"&amp;A1&amp;"radioButton1.isChecked()) answers["&amp;A1&amp;"]=1; else if (question"&amp;A1&amp;"radioButton2.isChecked()) answers["&amp;A1&amp;"]=2;"&amp;" else if (question"&amp;A1&amp;"radioButton3.isChecked()) answers["&amp;A1&amp;"]=3; else if (question"&amp;A1&amp;"radioButton4.isChecked()) answers["&amp;A1&amp;"]=4; else if (question"&amp;A1&amp;"radioButton5.isChecked()) answers["&amp;A1&amp;"]=5; else { notCompleted("&amp;A1&amp;", layout"&amp;A1&amp;"); return; }"</f>
+        <v>if (question1radioButton1.isChecked()) answers[1]=1; else if (question1radioButton2.isChecked()) answers[1]=2; else if (question1radioButton3.isChecked()) answers[1]=3; else if (question1radioButton4.isChecked()) answers[1]=4; else if (question1radioButton5.isChecked()) answers[1]=5; else { notCompleted(1, layout1); return; }</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="str">
+        <f t="shared" ref="B2:B50" si="0">"if (question"&amp;A2&amp;"radioButton1.isChecked()) answers["&amp;A2&amp;"]=1; else if (question"&amp;A2&amp;"radioButton2.isChecked()) answers["&amp;A2&amp;"]=2;"&amp;" else if (question"&amp;A2&amp;"radioButton3.isChecked()) answers["&amp;A2&amp;"]=3; else if (question"&amp;A2&amp;"radioButton4.isChecked()) answers["&amp;A2&amp;"]=4; else if (question"&amp;A2&amp;"radioButton5.isChecked()) answers["&amp;A2&amp;"]=5; else { notCompleted("&amp;A2&amp;", layout"&amp;A2&amp;"); return; }"</f>
+        <v>if (question2radioButton1.isChecked()) answers[2]=1; else if (question2radioButton2.isChecked()) answers[2]=2; else if (question2radioButton3.isChecked()) answers[2]=3; else if (question2radioButton4.isChecked()) answers[2]=4; else if (question2radioButton5.isChecked()) answers[2]=5; else { notCompleted(2, layout2); return; }</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question3radioButton1.isChecked()) answers[3]=1; else if (question3radioButton2.isChecked()) answers[3]=2; else if (question3radioButton3.isChecked()) answers[3]=3; else if (question3radioButton4.isChecked()) answers[3]=4; else if (question3radioButton5.isChecked()) answers[3]=5; else { notCompleted(3, layout3); return; }</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question4radioButton1.isChecked()) answers[4]=1; else if (question4radioButton2.isChecked()) answers[4]=2; else if (question4radioButton3.isChecked()) answers[4]=3; else if (question4radioButton4.isChecked()) answers[4]=4; else if (question4radioButton5.isChecked()) answers[4]=5; else { notCompleted(4, layout4); return; }</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question5radioButton1.isChecked()) answers[5]=1; else if (question5radioButton2.isChecked()) answers[5]=2; else if (question5radioButton3.isChecked()) answers[5]=3; else if (question5radioButton4.isChecked()) answers[5]=4; else if (question5radioButton5.isChecked()) answers[5]=5; else { notCompleted(5, layout5); return; }</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question6radioButton1.isChecked()) answers[6]=1; else if (question6radioButton2.isChecked()) answers[6]=2; else if (question6radioButton3.isChecked()) answers[6]=3; else if (question6radioButton4.isChecked()) answers[6]=4; else if (question6radioButton5.isChecked()) answers[6]=5; else { notCompleted(6, layout6); return; }</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question7radioButton1.isChecked()) answers[7]=1; else if (question7radioButton2.isChecked()) answers[7]=2; else if (question7radioButton3.isChecked()) answers[7]=3; else if (question7radioButton4.isChecked()) answers[7]=4; else if (question7radioButton5.isChecked()) answers[7]=5; else { notCompleted(7, layout7); return; }</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question8radioButton1.isChecked()) answers[8]=1; else if (question8radioButton2.isChecked()) answers[8]=2; else if (question8radioButton3.isChecked()) answers[8]=3; else if (question8radioButton4.isChecked()) answers[8]=4; else if (question8radioButton5.isChecked()) answers[8]=5; else { notCompleted(8, layout8); return; }</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question9radioButton1.isChecked()) answers[9]=1; else if (question9radioButton2.isChecked()) answers[9]=2; else if (question9radioButton3.isChecked()) answers[9]=3; else if (question9radioButton4.isChecked()) answers[9]=4; else if (question9radioButton5.isChecked()) answers[9]=5; else { notCompleted(9, layout9); return; }</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question10radioButton1.isChecked()) answers[10]=1; else if (question10radioButton2.isChecked()) answers[10]=2; else if (question10radioButton3.isChecked()) answers[10]=3; else if (question10radioButton4.isChecked()) answers[10]=4; else if (question10radioButton5.isChecked()) answers[10]=5; else { notCompleted(10, layout10); return; }</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question11radioButton1.isChecked()) answers[11]=1; else if (question11radioButton2.isChecked()) answers[11]=2; else if (question11radioButton3.isChecked()) answers[11]=3; else if (question11radioButton4.isChecked()) answers[11]=4; else if (question11radioButton5.isChecked()) answers[11]=5; else { notCompleted(11, layout11); return; }</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question12radioButton1.isChecked()) answers[12]=1; else if (question12radioButton2.isChecked()) answers[12]=2; else if (question12radioButton3.isChecked()) answers[12]=3; else if (question12radioButton4.isChecked()) answers[12]=4; else if (question12radioButton5.isChecked()) answers[12]=5; else { notCompleted(12, layout12); return; }</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question13radioButton1.isChecked()) answers[13]=1; else if (question13radioButton2.isChecked()) answers[13]=2; else if (question13radioButton3.isChecked()) answers[13]=3; else if (question13radioButton4.isChecked()) answers[13]=4; else if (question13radioButton5.isChecked()) answers[13]=5; else { notCompleted(13, layout13); return; }</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question14radioButton1.isChecked()) answers[14]=1; else if (question14radioButton2.isChecked()) answers[14]=2; else if (question14radioButton3.isChecked()) answers[14]=3; else if (question14radioButton4.isChecked()) answers[14]=4; else if (question14radioButton5.isChecked()) answers[14]=5; else { notCompleted(14, layout14); return; }</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question15radioButton1.isChecked()) answers[15]=1; else if (question15radioButton2.isChecked()) answers[15]=2; else if (question15radioButton3.isChecked()) answers[15]=3; else if (question15radioButton4.isChecked()) answers[15]=4; else if (question15radioButton5.isChecked()) answers[15]=5; else { notCompleted(15, layout15); return; }</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question16radioButton1.isChecked()) answers[16]=1; else if (question16radioButton2.isChecked()) answers[16]=2; else if (question16radioButton3.isChecked()) answers[16]=3; else if (question16radioButton4.isChecked()) answers[16]=4; else if (question16radioButton5.isChecked()) answers[16]=5; else { notCompleted(16, layout16); return; }</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question17radioButton1.isChecked()) answers[17]=1; else if (question17radioButton2.isChecked()) answers[17]=2; else if (question17radioButton3.isChecked()) answers[17]=3; else if (question17radioButton4.isChecked()) answers[17]=4; else if (question17radioButton5.isChecked()) answers[17]=5; else { notCompleted(17, layout17); return; }</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question18radioButton1.isChecked()) answers[18]=1; else if (question18radioButton2.isChecked()) answers[18]=2; else if (question18radioButton3.isChecked()) answers[18]=3; else if (question18radioButton4.isChecked()) answers[18]=4; else if (question18radioButton5.isChecked()) answers[18]=5; else { notCompleted(18, layout18); return; }</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question19radioButton1.isChecked()) answers[19]=1; else if (question19radioButton2.isChecked()) answers[19]=2; else if (question19radioButton3.isChecked()) answers[19]=3; else if (question19radioButton4.isChecked()) answers[19]=4; else if (question19radioButton5.isChecked()) answers[19]=5; else { notCompleted(19, layout19); return; }</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question20radioButton1.isChecked()) answers[20]=1; else if (question20radioButton2.isChecked()) answers[20]=2; else if (question20radioButton3.isChecked()) answers[20]=3; else if (question20radioButton4.isChecked()) answers[20]=4; else if (question20radioButton5.isChecked()) answers[20]=5; else { notCompleted(20, layout20); return; }</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question21radioButton1.isChecked()) answers[21]=1; else if (question21radioButton2.isChecked()) answers[21]=2; else if (question21radioButton3.isChecked()) answers[21]=3; else if (question21radioButton4.isChecked()) answers[21]=4; else if (question21radioButton5.isChecked()) answers[21]=5; else { notCompleted(21, layout21); return; }</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question22radioButton1.isChecked()) answers[22]=1; else if (question22radioButton2.isChecked()) answers[22]=2; else if (question22radioButton3.isChecked()) answers[22]=3; else if (question22radioButton4.isChecked()) answers[22]=4; else if (question22radioButton5.isChecked()) answers[22]=5; else { notCompleted(22, layout22); return; }</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question23radioButton1.isChecked()) answers[23]=1; else if (question23radioButton2.isChecked()) answers[23]=2; else if (question23radioButton3.isChecked()) answers[23]=3; else if (question23radioButton4.isChecked()) answers[23]=4; else if (question23radioButton5.isChecked()) answers[23]=5; else { notCompleted(23, layout23); return; }</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question24radioButton1.isChecked()) answers[24]=1; else if (question24radioButton2.isChecked()) answers[24]=2; else if (question24radioButton3.isChecked()) answers[24]=3; else if (question24radioButton4.isChecked()) answers[24]=4; else if (question24radioButton5.isChecked()) answers[24]=5; else { notCompleted(24, layout24); return; }</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question25radioButton1.isChecked()) answers[25]=1; else if (question25radioButton2.isChecked()) answers[25]=2; else if (question25radioButton3.isChecked()) answers[25]=3; else if (question25radioButton4.isChecked()) answers[25]=4; else if (question25radioButton5.isChecked()) answers[25]=5; else { notCompleted(25, layout25); return; }</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question26radioButton1.isChecked()) answers[26]=1; else if (question26radioButton2.isChecked()) answers[26]=2; else if (question26radioButton3.isChecked()) answers[26]=3; else if (question26radioButton4.isChecked()) answers[26]=4; else if (question26radioButton5.isChecked()) answers[26]=5; else { notCompleted(26, layout26); return; }</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question27radioButton1.isChecked()) answers[27]=1; else if (question27radioButton2.isChecked()) answers[27]=2; else if (question27radioButton3.isChecked()) answers[27]=3; else if (question27radioButton4.isChecked()) answers[27]=4; else if (question27radioButton5.isChecked()) answers[27]=5; else { notCompleted(27, layout27); return; }</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question28radioButton1.isChecked()) answers[28]=1; else if (question28radioButton2.isChecked()) answers[28]=2; else if (question28radioButton3.isChecked()) answers[28]=3; else if (question28radioButton4.isChecked()) answers[28]=4; else if (question28radioButton5.isChecked()) answers[28]=5; else { notCompleted(28, layout28); return; }</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question29radioButton1.isChecked()) answers[29]=1; else if (question29radioButton2.isChecked()) answers[29]=2; else if (question29radioButton3.isChecked()) answers[29]=3; else if (question29radioButton4.isChecked()) answers[29]=4; else if (question29radioButton5.isChecked()) answers[29]=5; else { notCompleted(29, layout29); return; }</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question30radioButton1.isChecked()) answers[30]=1; else if (question30radioButton2.isChecked()) answers[30]=2; else if (question30radioButton3.isChecked()) answers[30]=3; else if (question30radioButton4.isChecked()) answers[30]=4; else if (question30radioButton5.isChecked()) answers[30]=5; else { notCompleted(30, layout30); return; }</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question31radioButton1.isChecked()) answers[31]=1; else if (question31radioButton2.isChecked()) answers[31]=2; else if (question31radioButton3.isChecked()) answers[31]=3; else if (question31radioButton4.isChecked()) answers[31]=4; else if (question31radioButton5.isChecked()) answers[31]=5; else { notCompleted(31, layout31); return; }</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question32radioButton1.isChecked()) answers[32]=1; else if (question32radioButton2.isChecked()) answers[32]=2; else if (question32radioButton3.isChecked()) answers[32]=3; else if (question32radioButton4.isChecked()) answers[32]=4; else if (question32radioButton5.isChecked()) answers[32]=5; else { notCompleted(32, layout32); return; }</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question33radioButton1.isChecked()) answers[33]=1; else if (question33radioButton2.isChecked()) answers[33]=2; else if (question33radioButton3.isChecked()) answers[33]=3; else if (question33radioButton4.isChecked()) answers[33]=4; else if (question33radioButton5.isChecked()) answers[33]=5; else { notCompleted(33, layout33); return; }</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question34radioButton1.isChecked()) answers[34]=1; else if (question34radioButton2.isChecked()) answers[34]=2; else if (question34radioButton3.isChecked()) answers[34]=3; else if (question34radioButton4.isChecked()) answers[34]=4; else if (question34radioButton5.isChecked()) answers[34]=5; else { notCompleted(34, layout34); return; }</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question35radioButton1.isChecked()) answers[35]=1; else if (question35radioButton2.isChecked()) answers[35]=2; else if (question35radioButton3.isChecked()) answers[35]=3; else if (question35radioButton4.isChecked()) answers[35]=4; else if (question35radioButton5.isChecked()) answers[35]=5; else { notCompleted(35, layout35); return; }</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question36radioButton1.isChecked()) answers[36]=1; else if (question36radioButton2.isChecked()) answers[36]=2; else if (question36radioButton3.isChecked()) answers[36]=3; else if (question36radioButton4.isChecked()) answers[36]=4; else if (question36radioButton5.isChecked()) answers[36]=5; else { notCompleted(36, layout36); return; }</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question37radioButton1.isChecked()) answers[37]=1; else if (question37radioButton2.isChecked()) answers[37]=2; else if (question37radioButton3.isChecked()) answers[37]=3; else if (question37radioButton4.isChecked()) answers[37]=4; else if (question37radioButton5.isChecked()) answers[37]=5; else { notCompleted(37, layout37); return; }</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>38</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question38radioButton1.isChecked()) answers[38]=1; else if (question38radioButton2.isChecked()) answers[38]=2; else if (question38radioButton3.isChecked()) answers[38]=3; else if (question38radioButton4.isChecked()) answers[38]=4; else if (question38radioButton5.isChecked()) answers[38]=5; else { notCompleted(38, layout38); return; }</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>39</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question39radioButton1.isChecked()) answers[39]=1; else if (question39radioButton2.isChecked()) answers[39]=2; else if (question39radioButton3.isChecked()) answers[39]=3; else if (question39radioButton4.isChecked()) answers[39]=4; else if (question39radioButton5.isChecked()) answers[39]=5; else { notCompleted(39, layout39); return; }</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>40</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question40radioButton1.isChecked()) answers[40]=1; else if (question40radioButton2.isChecked()) answers[40]=2; else if (question40radioButton3.isChecked()) answers[40]=3; else if (question40radioButton4.isChecked()) answers[40]=4; else if (question40radioButton5.isChecked()) answers[40]=5; else { notCompleted(40, layout40); return; }</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question41radioButton1.isChecked()) answers[41]=1; else if (question41radioButton2.isChecked()) answers[41]=2; else if (question41radioButton3.isChecked()) answers[41]=3; else if (question41radioButton4.isChecked()) answers[41]=4; else if (question41radioButton5.isChecked()) answers[41]=5; else { notCompleted(41, layout41); return; }</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question42radioButton1.isChecked()) answers[42]=1; else if (question42radioButton2.isChecked()) answers[42]=2; else if (question42radioButton3.isChecked()) answers[42]=3; else if (question42radioButton4.isChecked()) answers[42]=4; else if (question42radioButton5.isChecked()) answers[42]=5; else { notCompleted(42, layout42); return; }</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>43</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B43" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question43radioButton1.isChecked()) answers[43]=1; else if (question43radioButton2.isChecked()) answers[43]=2; else if (question43radioButton3.isChecked()) answers[43]=3; else if (question43radioButton4.isChecked()) answers[43]=4; else if (question43radioButton5.isChecked()) answers[43]=5; else { notCompleted(43, layout43); return; }</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>44</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B44" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question44radioButton1.isChecked()) answers[44]=1; else if (question44radioButton2.isChecked()) answers[44]=2; else if (question44radioButton3.isChecked()) answers[44]=3; else if (question44radioButton4.isChecked()) answers[44]=4; else if (question44radioButton5.isChecked()) answers[44]=5; else { notCompleted(44, layout44); return; }</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>45</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B45" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question45radioButton1.isChecked()) answers[45]=1; else if (question45radioButton2.isChecked()) answers[45]=2; else if (question45radioButton3.isChecked()) answers[45]=3; else if (question45radioButton4.isChecked()) answers[45]=4; else if (question45radioButton5.isChecked()) answers[45]=5; else { notCompleted(45, layout45); return; }</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>46</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B46" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question46radioButton1.isChecked()) answers[46]=1; else if (question46radioButton2.isChecked()) answers[46]=2; else if (question46radioButton3.isChecked()) answers[46]=3; else if (question46radioButton4.isChecked()) answers[46]=4; else if (question46radioButton5.isChecked()) answers[46]=5; else { notCompleted(46, layout46); return; }</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>47</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B47" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question47radioButton1.isChecked()) answers[47]=1; else if (question47radioButton2.isChecked()) answers[47]=2; else if (question47radioButton3.isChecked()) answers[47]=3; else if (question47radioButton4.isChecked()) answers[47]=4; else if (question47radioButton5.isChecked()) answers[47]=5; else { notCompleted(47, layout47); return; }</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>48</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question48radioButton1.isChecked()) answers[48]=1; else if (question48radioButton2.isChecked()) answers[48]=2; else if (question48radioButton3.isChecked()) answers[48]=3; else if (question48radioButton4.isChecked()) answers[48]=4; else if (question48radioButton5.isChecked()) answers[48]=5; else { notCompleted(48, layout48); return; }</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>49</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question49radioButton1.isChecked()) answers[49]=1; else if (question49radioButton2.isChecked()) answers[49]=2; else if (question49radioButton3.isChecked()) answers[49]=3; else if (question49radioButton4.isChecked()) answers[49]=4; else if (question49radioButton5.isChecked()) answers[49]=5; else { notCompleted(49, layout49); return; }</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>50</v>
       </c>
+      <c r="B50" t="str">
+        <f t="shared" si="0"/>
+        <v>if (question50radioButton1.isChecked()) answers[50]=1; else if (question50radioButton2.isChecked()) answers[50]=2; else if (question50radioButton3.isChecked()) answers[50]=3; else if (question50radioButton4.isChecked()) answers[50]=4; else if (question50radioButton5.isChecked()) answers[50]=5; else { notCompleted(50, layout50); return; }</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="str">
+        <f>"layout"&amp;A1</f>
+        <v>layout1</v>
+      </c>
+      <c r="C1" t="str">
+        <f>"LinearLayout "&amp;B1&amp;" = new LinearLayout(this);"</f>
+        <v>LinearLayout layout1 = new LinearLayout(this);</v>
+      </c>
+      <c r="D1" t="str">
+        <f>B1&amp;" = findViewById(R.id."&amp;B1&amp;");"</f>
+        <v>layout1 = findViewById(R.id.layout1);</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="str">
+        <f t="shared" ref="B2:B50" si="0">"layout"&amp;A2</f>
+        <v>layout2</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C50" si="1">"LinearLayout "&amp;B2&amp;" = new LinearLayout(this);"</f>
+        <v>LinearLayout layout2 = new LinearLayout(this);</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D50" si="2">B2&amp;" = findViewById(R.id."&amp;B2&amp;");"</f>
+        <v>layout2 = findViewById(R.id.layout2);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" si="0"/>
+        <v>layout3</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout3 = new LinearLayout(this);</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="2"/>
+        <v>layout3 = findViewById(R.id.layout3);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>layout4</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout4 = new LinearLayout(this);</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="2"/>
+        <v>layout4 = findViewById(R.id.layout4);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>layout5</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout5 = new LinearLayout(this);</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="2"/>
+        <v>layout5 = findViewById(R.id.layout5);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>layout6</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout6 = new LinearLayout(this);</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="2"/>
+        <v>layout6 = findViewById(R.id.layout6);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>layout7</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout7 = new LinearLayout(this);</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="2"/>
+        <v>layout7 = findViewById(R.id.layout7);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>layout8</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout8 = new LinearLayout(this);</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="2"/>
+        <v>layout8 = findViewById(R.id.layout8);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>layout9</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout9 = new LinearLayout(this);</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="2"/>
+        <v>layout9 = findViewById(R.id.layout9);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>layout10</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout10 = new LinearLayout(this);</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="2"/>
+        <v>layout10 = findViewById(R.id.layout10);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>layout11</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout11 = new LinearLayout(this);</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="2"/>
+        <v>layout11 = findViewById(R.id.layout11);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>layout12</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout12 = new LinearLayout(this);</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="2"/>
+        <v>layout12 = findViewById(R.id.layout12);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>layout13</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout13 = new LinearLayout(this);</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="2"/>
+        <v>layout13 = findViewById(R.id.layout13);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>layout14</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout14 = new LinearLayout(this);</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="2"/>
+        <v>layout14 = findViewById(R.id.layout14);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>layout15</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout15 = new LinearLayout(this);</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="2"/>
+        <v>layout15 = findViewById(R.id.layout15);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>layout16</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout16 = new LinearLayout(this);</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="2"/>
+        <v>layout16 = findViewById(R.id.layout16);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>layout17</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout17 = new LinearLayout(this);</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="2"/>
+        <v>layout17 = findViewById(R.id.layout17);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>layout18</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout18 = new LinearLayout(this);</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="2"/>
+        <v>layout18 = findViewById(R.id.layout18);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>layout19</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout19 = new LinearLayout(this);</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="2"/>
+        <v>layout19 = findViewById(R.id.layout19);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>layout20</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout20 = new LinearLayout(this);</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="2"/>
+        <v>layout20 = findViewById(R.id.layout20);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>layout21</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout21 = new LinearLayout(this);</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="2"/>
+        <v>layout21 = findViewById(R.id.layout21);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>layout22</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout22 = new LinearLayout(this);</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="2"/>
+        <v>layout22 = findViewById(R.id.layout22);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>layout23</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout23 = new LinearLayout(this);</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="2"/>
+        <v>layout23 = findViewById(R.id.layout23);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>layout24</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout24 = new LinearLayout(this);</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="2"/>
+        <v>layout24 = findViewById(R.id.layout24);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>layout25</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout25 = new LinearLayout(this);</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="2"/>
+        <v>layout25 = findViewById(R.id.layout25);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>layout26</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout26 = new LinearLayout(this);</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="2"/>
+        <v>layout26 = findViewById(R.id.layout26);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>layout27</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout27 = new LinearLayout(this);</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="2"/>
+        <v>layout27 = findViewById(R.id.layout27);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>layout28</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout28 = new LinearLayout(this);</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="2"/>
+        <v>layout28 = findViewById(R.id.layout28);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>layout29</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout29 = new LinearLayout(this);</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="2"/>
+        <v>layout29 = findViewById(R.id.layout29);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>layout30</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout30 = new LinearLayout(this);</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="2"/>
+        <v>layout30 = findViewById(R.id.layout30);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>layout31</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout31 = new LinearLayout(this);</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="2"/>
+        <v>layout31 = findViewById(R.id.layout31);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>layout32</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout32 = new LinearLayout(this);</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="2"/>
+        <v>layout32 = findViewById(R.id.layout32);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>layout33</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout33 = new LinearLayout(this);</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="2"/>
+        <v>layout33 = findViewById(R.id.layout33);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>layout34</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout34 = new LinearLayout(this);</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="2"/>
+        <v>layout34 = findViewById(R.id.layout34);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>layout35</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout35 = new LinearLayout(this);</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="2"/>
+        <v>layout35 = findViewById(R.id.layout35);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>layout36</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout36 = new LinearLayout(this);</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="2"/>
+        <v>layout36 = findViewById(R.id.layout36);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>layout37</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout37 = new LinearLayout(this);</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="2"/>
+        <v>layout37 = findViewById(R.id.layout37);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>layout38</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout38 = new LinearLayout(this);</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="2"/>
+        <v>layout38 = findViewById(R.id.layout38);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>layout39</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout39 = new LinearLayout(this);</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="2"/>
+        <v>layout39 = findViewById(R.id.layout39);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>layout40</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout40 = new LinearLayout(this);</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="2"/>
+        <v>layout40 = findViewById(R.id.layout40);</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>layout41</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout41 = new LinearLayout(this);</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="2"/>
+        <v>layout41 = findViewById(R.id.layout41);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>layout42</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout42 = new LinearLayout(this);</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="2"/>
+        <v>layout42 = findViewById(R.id.layout42);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" si="0"/>
+        <v>layout43</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout43 = new LinearLayout(this);</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="2"/>
+        <v>layout43 = findViewById(R.id.layout43);</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" si="0"/>
+        <v>layout44</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout44 = new LinearLayout(this);</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="2"/>
+        <v>layout44 = findViewById(R.id.layout44);</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="0"/>
+        <v>layout45</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout45 = new LinearLayout(this);</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="2"/>
+        <v>layout45 = findViewById(R.id.layout45);</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="B46" t="str">
+        <f t="shared" si="0"/>
+        <v>layout46</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout46 = new LinearLayout(this);</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="2"/>
+        <v>layout46 = findViewById(R.id.layout46);</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>47</v>
+      </c>
+      <c r="B47" t="str">
+        <f t="shared" si="0"/>
+        <v>layout47</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout47 = new LinearLayout(this);</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="2"/>
+        <v>layout47 = findViewById(R.id.layout47);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" si="0"/>
+        <v>layout48</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout48 = new LinearLayout(this);</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="2"/>
+        <v>layout48 = findViewById(R.id.layout48);</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>49</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" si="0"/>
+        <v>layout49</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout49 = new LinearLayout(this);</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="2"/>
+        <v>layout49 = findViewById(R.id.layout49);</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>50</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" si="0"/>
+        <v>layout50</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="1"/>
+        <v>LinearLayout layout50 = new LinearLayout(this);</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="2"/>
+        <v>layout50 = findViewById(R.id.layout50);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add score calculation and graph java code
</commit_message>
<xml_diff>
--- a/_DESIGN/formulas.xlsx
+++ b/_DESIGN/formulas.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11415" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11415" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet4!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet4!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="79">
   <si>
     <t>&lt;LinearLayout                 android:layout_width="&amp;char(34)&amp;"match_parent"&amp;char(34)&amp;"                 android:layout_height="&amp;char(34)&amp;"match_parent"&amp;char(34)&amp;"                 android:orientation="&amp;char(34)&amp;"horizontal"&amp;char(34)&amp;"&gt;                  &lt;TextView                     android:id="&amp;char(34)&amp;"@+id/textView4"&amp;char(34)&amp;"                     android:layout_width="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                     android:layout_height="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                     android:layout_weight="&amp;char(34)&amp;"1"&amp;char(34)&amp;"                     android:text="&amp;char(34)&amp;"1."&amp;char(34)&amp;" /&gt;                  &lt;TextView                     android:id="&amp;char(34)&amp;"@+id/textView3"&amp;char(34)&amp;"                     android:layout_width="&amp;char(34)&amp;"183dp"&amp;char(34)&amp;"                     android:layout_height="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                     android:layout_weight="&amp;char(34)&amp;"1"&amp;char(34)&amp;"                     android:text="&amp;char(34)&amp;"TextView"&amp;char(34)&amp;" /&gt;                  &lt;RadioGroup                     android:layout_width="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                     android:layout_height="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                     android:layout_weight="&amp;char(34)&amp;"1"&amp;char(34)&amp;"                     android:orientation="&amp;char(34)&amp;"horizontal"&amp;char(34)&amp;"&gt;                      &lt;RadioButton                         android:id="&amp;char(34)&amp;"@+id/radioButton"&amp;char(34)&amp;"                         android:layout_width="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                         android:layout_height="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                         android:layout_weight="&amp;char(34)&amp;"1"&amp;char(34)&amp;" /&gt;                      &lt;RadioButton                         android:id="&amp;char(34)&amp;"@+id/radioButton2"&amp;char(34)&amp;"                         android:layout_width="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                         android:layout_height="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                         android:layout_weight="&amp;char(34)&amp;"1"&amp;char(34)&amp;" /&gt;                      &lt;RadioButton                         android:id="&amp;char(34)&amp;"@+id/radioButton3"&amp;char(34)&amp;"                         android:layout_width="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                         android:layout_height="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                         android:layout_weight="&amp;char(34)&amp;"1"&amp;char(34)&amp;" /&gt;                      &lt;RadioButton                         android:id="&amp;char(34)&amp;"@+id/radioButton4"&amp;char(34)&amp;"                         android:layout_width="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                         android:layout_height="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                         android:layout_weight="&amp;char(34)&amp;"1"&amp;char(34)&amp;" /&gt;                      &lt;RadioButton                         android:id="&amp;char(34)&amp;"@+id/radioButton5"&amp;char(34)&amp;"                         android:layout_width="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                         android:layout_height="&amp;char(34)&amp;"wrap_content"&amp;char(34)&amp;"                         android:layout_weight="&amp;char(34)&amp;"1"&amp;char(34)&amp;" /&gt;                 &lt;/RadioGroup&gt;              &lt;/LinearLayout&gt;</t>
   </si>
@@ -255,12 +256,27 @@
   <si>
     <t>if (question50radioButton1.isChecked()) answers[50]=1; else if (question50radioButton2.isChecked()) answers[50]=2; else if (question50radioButton3.isChecked()) answers[50]=3; else if (question50radioButton4.isChecked()) answers[50]=4; else if (question50radioButton5.isChecked()) answers[50]=5; else { notCompleted(50, layout50); return; }</t>
   </si>
+  <si>
+    <t>extraversion</t>
+  </si>
+  <si>
+    <t>agreeableness</t>
+  </si>
+  <si>
+    <t>conscientiousness</t>
+  </si>
+  <si>
+    <t>emotionalStability</t>
+  </si>
+  <si>
+    <t>intellectImagination</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,13 +290,25 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000080"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -295,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -310,11 +338,60 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -663,15 +740,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H56" sqref="H7:H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -687,11 +764,11 @@
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="5"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
@@ -707,11 +784,11 @@
       <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="5"/>
+      <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="1" t="s">
@@ -719,11 +796,11 @@
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="5"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="1" t="s">
@@ -731,27 +808,27 @@
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="5"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="5"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="1"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="5"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -2064,6 +2141,861 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="str">
+        <f>RIGHT(LEFT(B1,2),1)</f>
+        <v>1</v>
+      </c>
+      <c r="D1" t="str">
+        <f>LEFT(RIGHT(B1,2),1)</f>
+        <v>+</v>
+      </c>
+      <c r="E1" s="9">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:E50" si="0">RIGHT(LEFT(B2,2),1)</f>
+        <v>2</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D50" si="1">LEFT(RIGHT(B2,2),1)</f>
+        <v>-</v>
+      </c>
+      <c r="E2" s="9">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+      <c r="E3" s="9">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="E4" s="9">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+      <c r="E5" s="9">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D29" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D39" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D40" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D42" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>47</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D48" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>49</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D49" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>50</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D50" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>+</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="5">
+      <formula>NOT(ISERROR(SEARCH("5",C1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C50"/>
   <sheetViews>
@@ -2682,7 +3614,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I266"/>
   <sheetViews>
@@ -9273,7 +10205,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B52"/>
   <sheetViews>
@@ -9744,11 +10676,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>

</xml_diff>